<commit_message>
Third commit - here we can control the execution o fth testcases @ run time using I method interceptor
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/actitimetestdata.xlsx
+++ b/src/main/resources/excel/actitimetestdata.xlsx
@@ -8,64 +8,79 @@
   </bookViews>
   <sheets>
     <sheet name="runner" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>testcasename</t>
   </si>
   <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>logintest</t>
+  </si>
+  <si>
+    <t>VerifyActitimeVersion</t>
+  </si>
+  <si>
+    <t>verify the version</t>
+  </si>
+  <si>
+    <t>CreateUser</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>will create user</t>
+  </si>
+  <si>
     <t>execute</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>middlename</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>retrypassword</t>
+  </si>
+  <si>
+    <t>createusername</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>loginpassword</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>VerifyActitimeVersion</t>
-  </si>
-  <si>
-    <t>CreateUser</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>middlename</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>retrypassword</t>
-  </si>
-  <si>
-    <t>createusername</t>
-  </si>
-  <si>
-    <t>username</t>
   </si>
   <si>
     <t>admin</t>
@@ -94,10 +109,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -116,6 +131,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,15 +168,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,22 +185,31 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,32 +223,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,11 +238,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,7 +254,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,21 +262,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,187 +276,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,11 +472,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,6 +505,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,21 +559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -543,27 +567,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -576,127 +591,127 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1026,13 +1041,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="22.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="11.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1053,7 +1068,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1064,19 +1079,19 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1088,17 +1103,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="22.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="13.1428571428571" customWidth="1"/>
-    <col min="9" max="9" width="16.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1106,34 +1119,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1141,28 +1154,34 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1170,48 +1189,54 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>1223</v>
@@ -1220,13 +1245,83 @@
         <v>1223</v>
       </c>
       <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>